<commit_message>
Updated Plots, added robot data
</commit_message>
<xml_diff>
--- a/Data_Files/Logs/10 tan - Affect Trend.xlsx
+++ b/Data_Files/Logs/10 tan - Affect Trend.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="62">
   <si>
     <t>BV</t>
   </si>
@@ -160,6 +160,51 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>Emotions</t>
+  </si>
+  <si>
+    <t>happy</t>
+  </si>
+  <si>
+    <t>hope</t>
+  </si>
+  <si>
+    <t>sad</t>
+  </si>
+  <si>
+    <t>fear</t>
+  </si>
+  <si>
+    <t>anger</t>
+  </si>
+  <si>
+    <t>scared 1</t>
+  </si>
+  <si>
+    <t>scared 2</t>
+  </si>
+  <si>
+    <t>scared 3</t>
+  </si>
+  <si>
+    <t>Expressions</t>
+  </si>
+  <si>
+    <t>happy2</t>
+  </si>
+  <si>
+    <t>hope2</t>
+  </si>
+  <si>
+    <t>sad2</t>
+  </si>
+  <si>
+    <t>fear2</t>
+  </si>
+  <si>
+    <t>anger2</t>
   </si>
 </sst>
 </file>
@@ -859,8 +904,8 @@
               <c:numCache>
                 <c:formatCode>mm:ss</c:formatCode>
                 <c:ptCount val="92"/>
-                <c:pt idx="0" formatCode="m/d/yyyy\ h:mm:ss">
-                  <c:v>0.20729355324147036</c:v>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5.9930556744802743E-5</c:v>
@@ -1465,8 +1510,8 @@
               <c:numCache>
                 <c:formatCode>mm:ss</c:formatCode>
                 <c:ptCount val="92"/>
-                <c:pt idx="0" formatCode="m/d/yyyy\ h:mm:ss">
-                  <c:v>0.20729355324147036</c:v>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5.9930556744802743E-5</c:v>
@@ -2073,8 +2118,8 @@
               <c:numCache>
                 <c:formatCode>mm:ss</c:formatCode>
                 <c:ptCount val="92"/>
-                <c:pt idx="0" formatCode="m/d/yyyy\ h:mm:ss">
-                  <c:v>0.20729355324147036</c:v>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5.9930556744802743E-5</c:v>
@@ -2682,8 +2727,8 @@
               <c:numCache>
                 <c:formatCode>mm:ss</c:formatCode>
                 <c:ptCount val="92"/>
-                <c:pt idx="0" formatCode="m/d/yyyy\ h:mm:ss">
-                  <c:v>0.20729355324147036</c:v>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5.9930556744802743E-5</c:v>
@@ -3588,8 +3633,8 @@
               <c:numCache>
                 <c:formatCode>mm:ss</c:formatCode>
                 <c:ptCount val="92"/>
-                <c:pt idx="0" formatCode="m/d/yyyy\ h:mm:ss">
-                  <c:v>0.20729355324147036</c:v>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5.9930556744802743E-5</c:v>
@@ -4196,8 +4241,8 @@
               <c:numCache>
                 <c:formatCode>mm:ss</c:formatCode>
                 <c:ptCount val="92"/>
-                <c:pt idx="0" formatCode="m/d/yyyy\ h:mm:ss">
-                  <c:v>0.20729355324147036</c:v>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5.9930556744802743E-5</c:v>
@@ -4804,8 +4849,8 @@
               <c:numCache>
                 <c:formatCode>mm:ss</c:formatCode>
                 <c:ptCount val="92"/>
-                <c:pt idx="0" formatCode="m/d/yyyy\ h:mm:ss">
-                  <c:v>0.20729355324147036</c:v>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5.9930556744802743E-5</c:v>
@@ -5413,8 +5458,8 @@
               <c:numCache>
                 <c:formatCode>mm:ss</c:formatCode>
                 <c:ptCount val="92"/>
-                <c:pt idx="0" formatCode="m/d/yyyy\ h:mm:ss">
-                  <c:v>0.20729355324147036</c:v>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5.9930556744802743E-5</c:v>
@@ -6293,7 +6338,9 @@
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -6523,7 +6570,9 @@
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -9037,14 +9086,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M4" workbookViewId="0">
-      <selection activeCell="AE36" sqref="AE36"/>
+    <sheetView tabSelected="1" topLeftCell="N29" workbookViewId="0">
+      <selection activeCell="Z44" sqref="Z44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" customWidth="1"/>
+    <col min="2" max="2" width="7.77734375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.21875" customWidth="1"/>
     <col min="31" max="31" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="7.33203125" bestFit="1" customWidth="1"/>
@@ -9117,9 +9166,9 @@
       <c r="A2" s="2">
         <v>42411.692293553242</v>
       </c>
-      <c r="B2" s="2">
-        <f>A2-AE$2</f>
-        <v>0.20729355324147036</v>
+      <c r="B2" s="3">
+        <f>A2-A$2</f>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -11121,7 +11170,7 @@
       </c>
       <c r="P32" s="1"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>42411.694633460647</v>
       </c>
@@ -11168,7 +11217,7 @@
       </c>
       <c r="P33" s="1"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>42411.694697488427</v>
       </c>
@@ -11215,7 +11264,7 @@
       </c>
       <c r="P34" s="1"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>42411.694757476849</v>
       </c>
@@ -11262,7 +11311,7 @@
       </c>
       <c r="P35" s="1"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>42411.694821504629</v>
       </c>
@@ -11309,7 +11358,7 @@
       </c>
       <c r="P36" s="1"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>42411.694886053243</v>
       </c>
@@ -11355,8 +11404,26 @@
         <v>0.95652173913043481</v>
       </c>
       <c r="P37" s="1"/>
+      <c r="Q37" t="s">
+        <v>47</v>
+      </c>
+      <c r="R37">
+        <v>0</v>
+      </c>
+      <c r="S37" t="s">
+        <v>48</v>
+      </c>
+      <c r="U37" t="s">
+        <v>56</v>
+      </c>
+      <c r="V37">
+        <v>0</v>
+      </c>
+      <c r="W37" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>42411.694946203701</v>
       </c>
@@ -11402,8 +11469,20 @@
         <v>0.95652173913043481</v>
       </c>
       <c r="P38" s="1"/>
+      <c r="R38">
+        <v>1</v>
+      </c>
+      <c r="S38" t="s">
+        <v>49</v>
+      </c>
+      <c r="V38">
+        <v>1</v>
+      </c>
+      <c r="W38" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>42411.695005914349</v>
       </c>
@@ -11449,8 +11528,20 @@
         <v>0.95652173913043481</v>
       </c>
       <c r="P39" s="1"/>
+      <c r="R39">
+        <v>2</v>
+      </c>
+      <c r="S39" t="s">
+        <v>50</v>
+      </c>
+      <c r="V39">
+        <v>2</v>
+      </c>
+      <c r="W39" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>42411.695065810185</v>
       </c>
@@ -11496,8 +11587,20 @@
         <v>0.95652173913043481</v>
       </c>
       <c r="P40" s="1"/>
+      <c r="R40">
+        <v>3</v>
+      </c>
+      <c r="S40" t="s">
+        <v>51</v>
+      </c>
+      <c r="V40">
+        <v>3</v>
+      </c>
+      <c r="W40" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>42411.695125497688</v>
       </c>
@@ -11543,8 +11646,20 @@
         <v>0.95652173913043481</v>
       </c>
       <c r="P41" s="1"/>
+      <c r="R41">
+        <v>4</v>
+      </c>
+      <c r="S41" t="s">
+        <v>52</v>
+      </c>
+      <c r="V41">
+        <v>4</v>
+      </c>
+      <c r="W41" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>42411.695189293983</v>
       </c>
@@ -11590,8 +11705,20 @@
         <v>0.95652173913043481</v>
       </c>
       <c r="P42" s="1"/>
+      <c r="R42">
+        <v>5</v>
+      </c>
+      <c r="S42" t="s">
+        <v>53</v>
+      </c>
+      <c r="V42">
+        <v>5</v>
+      </c>
+      <c r="W42" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>42411.695253333331</v>
       </c>
@@ -11637,8 +11764,20 @@
         <v>0.95652173913043481</v>
       </c>
       <c r="P43" s="1"/>
+      <c r="R43">
+        <v>6</v>
+      </c>
+      <c r="S43" t="s">
+        <v>54</v>
+      </c>
+      <c r="V43">
+        <v>6</v>
+      </c>
+      <c r="W43" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>42411.695313263888</v>
       </c>
@@ -11683,8 +11822,20 @@
         <f>AVERAGE(Table1[MA])</f>
         <v>0.95652173913043481</v>
       </c>
+      <c r="R44">
+        <v>7</v>
+      </c>
+      <c r="S44" t="s">
+        <v>55</v>
+      </c>
+      <c r="V44">
+        <v>7</v>
+      </c>
+      <c r="W44" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>42411.695373229166</v>
       </c>
@@ -11729,8 +11880,14 @@
         <f>AVERAGE(Table1[MA])</f>
         <v>0.95652173913043481</v>
       </c>
+      <c r="V45">
+        <v>8</v>
+      </c>
+      <c r="W45" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>42411.695435000001</v>
       </c>
@@ -11775,8 +11932,14 @@
         <f>AVERAGE(Table1[MA])</f>
         <v>0.95652173913043481</v>
       </c>
+      <c r="V46">
+        <v>9</v>
+      </c>
+      <c r="W46" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>42411.695495127315</v>
       </c>
@@ -11821,8 +11984,14 @@
         <f>AVERAGE(Table1[MA])</f>
         <v>0.95652173913043481</v>
       </c>
+      <c r="V47">
+        <v>10</v>
+      </c>
+      <c r="W47" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>42411.695561053239</v>
       </c>
@@ -11867,8 +12036,14 @@
         <f>AVERAGE(Table1[MA])</f>
         <v>0.95652173913043481</v>
       </c>
+      <c r="V48">
+        <v>11</v>
+      </c>
+      <c r="W48" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>42411.695623368054</v>
       </c>
@@ -11913,8 +12088,14 @@
         <f>AVERAGE(Table1[MA])</f>
         <v>0.95652173913043481</v>
       </c>
+      <c r="V49">
+        <v>12</v>
+      </c>
+      <c r="W49" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>42411.695683171296</v>
       </c>
@@ -11960,7 +12141,7 @@
         <v>0.95652173913043481</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>42411.695743194447</v>
       </c>
@@ -12006,7 +12187,7 @@
         <v>0.95652173913043481</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>42411.695807187498</v>
       </c>
@@ -12052,7 +12233,7 @@
         <v>0.95652173913043481</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>42411.695871481483</v>
       </c>
@@ -12098,7 +12279,7 @@
         <v>0.95652173913043481</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>42411.695935995369</v>
       </c>
@@ -12144,7 +12325,7 @@
         <v>0.95652173913043481</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>42411.696000219905</v>
       </c>
@@ -12190,7 +12371,7 @@
         <v>0.95652173913043481</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>42411.696060520837</v>
       </c>
@@ -12236,7 +12417,7 @@
         <v>0.95652173913043481</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>42411.696122499998</v>
       </c>
@@ -12282,7 +12463,7 @@
         <v>0.95652173913043481</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>42411.696182847219</v>
       </c>
@@ -12328,7 +12509,7 @@
         <v>0.95652173913043481</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>42411.696246898151</v>
       </c>
@@ -12374,7 +12555,7 @@
         <v>0.95652173913043481</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>42411.696307071761</v>
       </c>
@@ -12420,7 +12601,7 @@
         <v>0.95652173913043481</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>42411.696367141201</v>
       </c>
@@ -12466,7 +12647,7 @@
         <v>0.95652173913043481</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>42411.696427314811</v>
       </c>
@@ -12512,7 +12693,7 @@
         <v>0.95652173913043481</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>42411.696491261573</v>
       </c>
@@ -12558,7 +12739,7 @@
         <v>0.95652173913043481</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>42411.696551388886</v>
       </c>

</xml_diff>